<commit_message>
copy formatting from previous cell
</commit_message>
<xml_diff>
--- a/tests/data/input.xlsx
+++ b/tests/data/input.xlsx
@@ -66,7 +66,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0">
+    <comment ref="E1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">datetime</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -80,7 +93,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0">
+    <comment ref="L1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -93,7 +106,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0">
+    <comment ref="M1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -106,7 +119,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0">
+    <comment ref="N1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -119,7 +132,21 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0">
+    <comment ref="P1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">sensor.mysensor
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -132,7 +159,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0">
+    <comment ref="S1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -150,7 +177,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -161,6 +188,9 @@
     <t xml:space="preserve">Time</t>
   </si>
   <si>
+    <t xml:space="preserve">Formatted Date</t>
+  </si>
+  <si>
     <t xml:space="preserve">My Entity</t>
   </si>
   <si>
@@ -179,10 +209,13 @@
     <t xml:space="preserve">My-Float</t>
   </si>
   <si>
-    <t xml:space="preserve">My-Unknown</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unknown</t>
+    <t xml:space="preserve">Euro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unknown Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unknown Entity</t>
   </si>
   <si>
     <t xml:space="preserve">Header 1</t>
@@ -201,12 +234,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="7">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
     <numFmt numFmtId="167" formatCode="hh:mm:ss"/>
     <numFmt numFmtId="168" formatCode="0.00"/>
+    <numFmt numFmtId="169" formatCode="#,##0.00\ [$€-407];[RED]\-#,##0.00\ [$€-407]"/>
+    <numFmt numFmtId="170" formatCode="dd/mm/yyyy\ hh:m"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -273,7 +308,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -294,6 +329,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -311,6 +350,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -331,65 +378,86 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
+      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="19.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="9.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="4" width="6.76"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="9" style="4" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="10" style="4" width="11.57"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="16.94"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="4" width="6.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="4" width="10.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="4" width="6.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="4" width="8.61"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="15" min="15" style="4" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="5" width="6.94"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="17" min="17" style="4" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="4" width="14.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="14.72"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="8"/>
+      <c r="E1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8"/>
+      <c r="G1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="I1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="P1" s="11" t="s">
         <v>10</v>
+      </c>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="S1" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D2" s="8" t="n">
+      <c r="G2" s="9" t="n">
         <v>21</v>
       </c>
-      <c r="F2" s="9" t="n">
-        <f aca="false">D2/2</f>
+      <c r="I2" s="10" t="n">
+        <f aca="false">G2/2</f>
         <v>10.5</v>
+      </c>
+      <c r="P2" s="5" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -402,16 +470,22 @@
       <c r="C3" s="3" t="n">
         <v>0.522916666666667</v>
       </c>
-      <c r="D3" s="8" t="n">
+      <c r="E3" s="12" t="n">
+        <v>45215.6111111111</v>
+      </c>
+      <c r="G3" s="9" t="n">
         <v>42</v>
       </c>
-      <c r="F3" s="4" t="n">
-        <f aca="false">D3/2</f>
+      <c r="I3" s="4" t="n">
+        <f aca="false">G3/2</f>
         <v>21</v>
       </c>
-      <c r="G3" s="9" t="n">
-        <f aca="false">D3-D2</f>
+      <c r="J3" s="10" t="n">
+        <f aca="false">G3-G2</f>
         <v>21</v>
+      </c>
+      <c r="P3" s="5" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -437,7 +511,7 @@
       <selection pane="topLeft" activeCell="K19" activeCellId="0" sqref="K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -460,22 +534,22 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>12</v>
+      <c r="A1" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>14</v>
+      <c r="A2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>